<commit_message>
Update IG file path in ig.ini 87bfcdde51d9439738e2a8b21aac411aab0d0a38
</commit_message>
<xml_diff>
--- a/main/ig/CodeSystem-competence-code-system.xlsx
+++ b/main/ig/CodeSystem-competence-code-system.xlsx
@@ -24,7 +24,7 @@
     <t>URL</t>
   </si>
   <si>
-    <t>https://interop.esante.gouv.fr/ig/fhir/[code]/CodeSystem/competence-code-system</t>
+    <t>https://interop.esante.gouv.fr/ig/fhir/ruim/CodeSystem/competence-code-system</t>
   </si>
   <si>
     <t>Version</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2026-01-29T17:15:36+00:00</t>
+    <t>2026-02-06T10:39:27+00:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>